<commit_message>
Cambios al archivo PBI y ajustes catálogo
</commit_message>
<xml_diff>
--- a/Catálogos data/partidos_mundial_2026.xlsx
+++ b/Catálogos data/partidos_mundial_2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tareas\Programación\Análisis de datos\Preanálisis mundial 2026\Catálogos data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A68D8AFA-589F-4481-878B-4B70E18D8169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAF365B-2BF3-471B-A69B-9E593121BA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5DEC00DC-9375-4565-8422-5F3CD4421EEB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
   <si>
     <t>mes</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>GDL</t>
-  </si>
-  <si>
-    <t>Corsea del Sur</t>
   </si>
   <si>
     <t>Uruguay</t>
@@ -442,7 +439,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +494,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -539,10 +536,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -556,7 +553,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -567,10 +564,10 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
         <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -584,7 +581,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -595,13 +592,13 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
         <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -609,13 +606,13 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -626,10 +623,10 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -643,7 +640,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>